<commit_message>
fix project name of TestViewPoint_Register
</commit_message>
<xml_diff>
--- a/WIP/Users/LucPT/FAP_TestViewpoint_Register_v1.0_EN.xlsx
+++ b/WIP/Users/LucPT/FAP_TestViewpoint_Register_v1.0_EN.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\admin-pc\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\2015SUMJS01\WIP\Users\LucPT\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="135" windowWidth="11760" windowHeight="5490" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="135" windowWidth="11760" windowHeight="5490"/>
   </bookViews>
   <sheets>
     <sheet name="Cover" sheetId="1" r:id="rId1"/>
@@ -556,7 +556,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="178">
   <si>
     <t>SST Test viewpoint</t>
   </si>
@@ -991,9 +991,6 @@
     <t>Chỉ tiêu thể hiện là đang phù hợp ở mức độ như thế nào trong quy cách・quy tắc・tiêu chuẩn (của protocol v.v…)liên quan đến tính linh động</t>
   </si>
   <si>
-    <t xml:space="preserve">USEFUL JAPANESE DICTIONARY FOR VIETNAMESE </t>
-  </si>
-  <si>
     <t>Password</t>
   </si>
   <si>
@@ -1084,9 +1081,6 @@
     <t>LucPTSE02923</t>
   </si>
   <si>
-    <t>15/7/2015</t>
-  </si>
-  <si>
     <t>FAP</t>
   </si>
   <si>
@@ -1130,6 +1124,9 @@
   </si>
   <si>
     <t>ReInput password in "Confirm Password" textbox</t>
+  </si>
+  <si>
+    <t>Fly Away Plus</t>
   </si>
 </sst>
 </file>
@@ -3129,6 +3126,24 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="3" borderId="10" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3149,24 +3164,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="23" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="24" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="21" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="64" fillId="30" borderId="30" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -6296,8 +6293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H16"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -6316,14 +6313,14 @@
     <row r="2" spans="1:8" s="5" customFormat="1" ht="75.75" customHeight="1">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
-      <c r="C2" s="103" t="s">
+      <c r="C2" s="109" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="103"/>
-      <c r="E2" s="103"/>
-      <c r="F2" s="103"/>
-      <c r="G2" s="103"/>
-      <c r="H2" s="104"/>
+      <c r="D2" s="109"/>
+      <c r="E2" s="109"/>
+      <c r="F2" s="109"/>
+      <c r="G2" s="109"/>
+      <c r="H2" s="110"/>
     </row>
     <row r="3" spans="1:8" ht="15" customHeight="1">
       <c r="B3" s="6"/>
@@ -6338,57 +6335,57 @@
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="105" t="s">
-        <v>134</v>
-      </c>
-      <c r="D4" s="105"/>
-      <c r="E4" s="105"/>
-      <c r="F4" s="105"/>
+      <c r="C4" s="111" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="111"/>
+      <c r="E4" s="111"/>
+      <c r="F4" s="111"/>
       <c r="G4" s="12" t="s">
         <v>2</v>
       </c>
       <c r="H4" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="14.25" customHeight="1">
       <c r="B5" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="105" t="s">
-        <v>164</v>
-      </c>
-      <c r="D5" s="105"/>
-      <c r="E5" s="105"/>
-      <c r="F5" s="105"/>
+      <c r="C5" s="111" t="s">
+        <v>162</v>
+      </c>
+      <c r="D5" s="111"/>
+      <c r="E5" s="111"/>
+      <c r="F5" s="111"/>
       <c r="G5" s="12" t="s">
         <v>4</v>
       </c>
       <c r="H5" s="13"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" customHeight="1">
-      <c r="B6" s="106" t="s">
+      <c r="B6" s="112" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="107" t="s">
-        <v>165</v>
-      </c>
-      <c r="D6" s="107"/>
-      <c r="E6" s="107"/>
-      <c r="F6" s="107"/>
+      <c r="C6" s="113" t="s">
+        <v>163</v>
+      </c>
+      <c r="D6" s="113"/>
+      <c r="E6" s="113"/>
+      <c r="F6" s="113"/>
       <c r="G6" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="H6" s="14" t="s">
-        <v>163</v>
+      <c r="H6" s="14">
+        <v>42345</v>
       </c>
     </row>
     <row r="7" spans="1:8" ht="13.5" customHeight="1">
-      <c r="B7" s="106"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
+      <c r="B7" s="112"/>
+      <c r="C7" s="113"/>
+      <c r="D7" s="113"/>
+      <c r="E7" s="113"/>
+      <c r="F7" s="113"/>
       <c r="G7" s="12" t="s">
         <v>7</v>
       </c>
@@ -6411,10 +6408,10 @@
       <c r="B9" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="101" t="s">
+      <c r="C9" s="107" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="102"/>
+      <c r="D9" s="108"/>
       <c r="E9" s="19" t="s">
         <v>11</v>
       </c>
@@ -6429,13 +6426,13 @@
       </c>
     </row>
     <row r="10" spans="1:8" s="21" customFormat="1" ht="25.5">
-      <c r="B10" s="22" t="s">
-        <v>163</v>
-      </c>
-      <c r="C10" s="110" t="s">
+      <c r="B10" s="22">
+        <v>42345</v>
+      </c>
+      <c r="C10" s="103" t="s">
         <v>8</v>
       </c>
-      <c r="D10" s="111"/>
+      <c r="D10" s="104"/>
       <c r="E10" s="23" t="s">
         <v>15</v>
       </c>
@@ -6444,13 +6441,13 @@
         <v>16</v>
       </c>
       <c r="H10" s="26" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:8" s="21" customFormat="1" ht="13.5" customHeight="1">
       <c r="B11" s="27"/>
-      <c r="C11" s="110"/>
-      <c r="D11" s="111"/>
+      <c r="C11" s="103"/>
+      <c r="D11" s="104"/>
       <c r="E11" s="23"/>
       <c r="F11" s="24"/>
       <c r="G11" s="25"/>
@@ -6458,8 +6455,8 @@
     </row>
     <row r="12" spans="1:8" s="21" customFormat="1">
       <c r="B12" s="29"/>
-      <c r="C12" s="112"/>
-      <c r="D12" s="113"/>
+      <c r="C12" s="105"/>
+      <c r="D12" s="106"/>
       <c r="E12" s="30"/>
       <c r="F12" s="24"/>
       <c r="G12" s="25"/>
@@ -6467,8 +6464,8 @@
     </row>
     <row r="13" spans="1:8" s="21" customFormat="1">
       <c r="B13" s="29"/>
-      <c r="C13" s="110"/>
-      <c r="D13" s="111"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="104"/>
       <c r="E13" s="30"/>
       <c r="F13" s="24"/>
       <c r="G13" s="31"/>
@@ -6476,8 +6473,8 @@
     </row>
     <row r="14" spans="1:8" s="21" customFormat="1">
       <c r="B14" s="29"/>
-      <c r="C14" s="110"/>
-      <c r="D14" s="111"/>
+      <c r="C14" s="103"/>
+      <c r="D14" s="104"/>
       <c r="E14" s="30"/>
       <c r="F14" s="24"/>
       <c r="G14" s="24"/>
@@ -6485,8 +6482,8 @@
     </row>
     <row r="15" spans="1:8" s="21" customFormat="1">
       <c r="B15" s="29"/>
-      <c r="C15" s="110"/>
-      <c r="D15" s="111"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="104"/>
       <c r="E15" s="30"/>
       <c r="F15" s="24"/>
       <c r="G15" s="24"/>
@@ -6494,8 +6491,8 @@
     </row>
     <row r="16" spans="1:8" ht="13.5" thickBot="1">
       <c r="B16" s="32"/>
-      <c r="C16" s="108"/>
-      <c r="D16" s="109"/>
+      <c r="C16" s="101"/>
+      <c r="D16" s="102"/>
       <c r="E16" s="33"/>
       <c r="F16" s="34"/>
       <c r="G16" s="35"/>
@@ -6503,6 +6500,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C2:H2"/>
+    <mergeCell ref="C4:F4"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="C6:F7"/>
     <mergeCell ref="C16:D16"/>
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:D11"/>
@@ -6510,12 +6513,6 @@
     <mergeCell ref="C13:D13"/>
     <mergeCell ref="C14:D14"/>
     <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C2:H2"/>
-    <mergeCell ref="C4:F4"/>
-    <mergeCell ref="C5:F5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="C6:F7"/>
   </mergeCells>
   <pageMargins left="0.47013888888888888" right="0.47013888888888888" top="0.5" bottom="0.35138888888888886" header="0.51180555555555562" footer="0.1701388888888889"/>
   <pageSetup paperSize="9" firstPageNumber="0" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -6531,7 +6528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M118"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+    <sheetView showGridLines="0" view="pageBreakPreview" topLeftCell="A16" zoomScale="85" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
       <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
@@ -6653,7 +6650,7 @@
         <v>1</v>
       </c>
       <c r="D6" s="42" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="E6" s="43"/>
       <c r="F6" s="43"/>
@@ -6725,7 +6722,7 @@
         <v>38</v>
       </c>
       <c r="L9" s="59" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:12" s="44" customFormat="1" ht="98.25" customHeight="1">
@@ -6753,7 +6750,7 @@
         <v>41</v>
       </c>
       <c r="L10" s="59" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:12" s="44" customFormat="1" ht="21.75" customHeight="1">
@@ -6783,7 +6780,7 @@
       <c r="D12" s="60"/>
       <c r="E12" s="61"/>
       <c r="F12" s="51" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G12" s="52"/>
       <c r="H12" s="52"/>
@@ -6802,7 +6799,7 @@
       <c r="E13" s="56"/>
       <c r="F13" s="62"/>
       <c r="G13" s="62" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="H13" s="49" t="s">
         <v>35</v>
@@ -6814,10 +6811,10 @@
         <v>37</v>
       </c>
       <c r="K13" s="56" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="L13" s="62" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="14" spans="1:12" s="44" customFormat="1" ht="46.5" customHeight="1">
@@ -6830,7 +6827,7 @@
       <c r="E14" s="56"/>
       <c r="F14" s="62"/>
       <c r="G14" s="62" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="H14" s="49" t="s">
         <v>35</v>
@@ -6842,10 +6839,10 @@
         <v>37</v>
       </c>
       <c r="K14" s="56" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="L14" s="62" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="15" spans="1:12" s="44" customFormat="1" ht="42" customHeight="1">
@@ -6858,7 +6855,7 @@
       <c r="E15" s="64"/>
       <c r="F15" s="63"/>
       <c r="G15" s="63" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="H15" s="49" t="s">
         <v>35</v>
@@ -6870,10 +6867,10 @@
         <v>37</v>
       </c>
       <c r="K15" s="56" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="L15" s="62" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="16" spans="1:12" s="44" customFormat="1" ht="34.5" customHeight="1">
@@ -6886,7 +6883,7 @@
       <c r="E16" s="64"/>
       <c r="F16" s="63"/>
       <c r="G16" s="63" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="H16" s="49" t="s">
         <v>35</v>
@@ -6898,23 +6895,23 @@
         <v>37</v>
       </c>
       <c r="K16" s="59" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="L16" s="56" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="17" spans="1:12" s="44" customFormat="1" ht="31.5" customHeight="1">
       <c r="A17" s="47"/>
       <c r="B17" s="48"/>
       <c r="C17" s="49" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D17" s="60"/>
       <c r="E17" s="64"/>
       <c r="F17" s="63"/>
       <c r="G17" s="63" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="H17" s="49" t="s">
         <v>35</v>
@@ -6926,23 +6923,23 @@
         <v>37</v>
       </c>
       <c r="K17" s="59" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="L17" s="56" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="18" spans="1:12" s="44" customFormat="1" ht="30" customHeight="1">
       <c r="A18" s="47"/>
       <c r="B18" s="48"/>
       <c r="C18" s="49" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D18" s="60"/>
       <c r="E18" s="64"/>
       <c r="F18" s="63"/>
       <c r="G18" s="63" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="H18" s="49" t="s">
         <v>35</v>
@@ -6954,23 +6951,23 @@
         <v>37</v>
       </c>
       <c r="K18" s="59" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L18" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="19" spans="1:12" s="44" customFormat="1" ht="30" customHeight="1">
       <c r="A19" s="47"/>
       <c r="B19" s="48"/>
       <c r="C19" s="49" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="D19" s="60"/>
       <c r="E19" s="64"/>
       <c r="F19" s="63"/>
       <c r="G19" s="63" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="H19" s="49" t="s">
         <v>35</v>
@@ -6982,23 +6979,23 @@
         <v>37</v>
       </c>
       <c r="K19" s="59" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="L19" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="20" spans="1:12" s="44" customFormat="1" ht="30" customHeight="1">
       <c r="A20" s="47"/>
       <c r="B20" s="48"/>
       <c r="C20" s="49" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D20" s="60"/>
       <c r="E20" s="64"/>
       <c r="F20" s="63"/>
       <c r="G20" s="63" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="H20" s="49" t="s">
         <v>35</v>
@@ -7010,23 +7007,23 @@
         <v>37</v>
       </c>
       <c r="K20" s="59" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L20" s="56" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="21" spans="1:12" s="44" customFormat="1" ht="30" customHeight="1">
       <c r="A21" s="47"/>
       <c r="B21" s="48"/>
       <c r="C21" s="49" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="D21" s="60"/>
       <c r="E21" s="64"/>
       <c r="F21" s="63"/>
       <c r="G21" s="63" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="H21" s="49" t="s">
         <v>35</v>
@@ -7038,23 +7035,23 @@
         <v>37</v>
       </c>
       <c r="K21" s="59" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="L21" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="22" spans="1:12" s="44" customFormat="1" ht="30" customHeight="1">
       <c r="A22" s="47"/>
       <c r="B22" s="48"/>
       <c r="C22" s="49" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D22" s="60"/>
       <c r="E22" s="64"/>
       <c r="F22" s="63"/>
       <c r="G22" s="63" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H22" s="49" t="s">
         <v>35</v>
@@ -7066,10 +7063,10 @@
         <v>37</v>
       </c>
       <c r="K22" s="59" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="L22" s="56" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="23" spans="1:12" s="44" customFormat="1" ht="38.25" customHeight="1">
@@ -7081,7 +7078,7 @@
       <c r="D23" s="60"/>
       <c r="E23" s="61"/>
       <c r="F23" s="51" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G23" s="52"/>
       <c r="H23" s="52"/>
@@ -7100,7 +7097,7 @@
       <c r="E24" s="63"/>
       <c r="F24" s="56"/>
       <c r="G24" s="56" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="H24" s="49" t="s">
         <v>35</v>
@@ -7112,10 +7109,10 @@
         <v>37</v>
       </c>
       <c r="K24" s="59" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L24" s="56" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:12" s="44" customFormat="1" ht="33" customHeight="1">
@@ -7132,10 +7129,10 @@
       <c r="I25" s="57"/>
       <c r="J25" s="58"/>
       <c r="K25" s="59" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="L25" s="56" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:12" s="44" customFormat="1">
@@ -8246,7 +8243,7 @@
   <sheetData>
     <row r="2" spans="1:1" ht="15">
       <c r="A2" s="80" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>